<commit_message>
Updated code with latest main and fixed TokenManager
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/Team05-APISquadTestData.xlsx
+++ b/src/test/resources/TestData/Team05-APISquadTestData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dineshdeshmukh/eclipse-workspace/Team05APISquadHackathon/src/test/resources/TestData/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41F5CBDB-819B-EE45-BD92-A5044FDB4E6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB8F5CAA-4847-D34A-A6B9-FA2024144D47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="45460" yWindow="-2960" windowWidth="23260" windowHeight="18240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="19980" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="923" uniqueCount="312">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="951" uniqueCount="325">
   <si>
     <t>ScenarioName</t>
   </si>
@@ -768,9 +768,6 @@
     <t>Admin@123</t>
   </si>
   <si>
-    <t>invalid password</t>
-  </si>
-  <si>
     <t>dhuruvalak01@gmail.com</t>
   </si>
   <si>
@@ -801,16 +798,7 @@
     <t>invalid endpoint</t>
   </si>
   <si>
-    <t>invalid base url</t>
-  </si>
-  <si>
-    <t>invalid content type</t>
-  </si>
-  <si>
     <t>application/jsonnn</t>
-  </si>
-  <si>
-    <t>invalid method</t>
   </si>
   <si>
     <t>valid email</t>
@@ -962,12 +950,63 @@
   <si>
     <t>logoutlms</t>
   </si>
+  <si>
+    <t>numbers in email</t>
+  </si>
+  <si>
+    <t>Team5@USA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">invalid content </t>
+  </si>
+  <si>
+    <t>invalid base URL</t>
+  </si>
+  <si>
+    <t>loginn</t>
+  </si>
+  <si>
+    <t>$#%%^&amp;@gmailcom</t>
+  </si>
+  <si>
+    <t>123456@gmail.com</t>
+  </si>
+  <si>
+    <t>/login/forgotpassword/confirmEmaill</t>
+  </si>
+  <si>
+    <t>Bearer Token</t>
+  </si>
+  <si>
+    <t>No Auth</t>
+  </si>
+  <si>
+    <t>invalid method</t>
+  </si>
+  <si>
+    <t>numbers in password</t>
+  </si>
+  <si>
+    <t>GET method test</t>
+  </si>
+  <si>
+    <t>invalid content</t>
+  </si>
+  <si>
+    <t>InvalidJason</t>
+  </si>
+  <si>
+    <t>special chars in confirmEmail</t>
+  </si>
+  <si>
+    <t>Team5@USAA3</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="22" x14ac:knownFonts="1">
+  <fonts count="23" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1118,6 +1157,11 @@
       <name val="Consolas"/>
       <family val="3"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="4"/>
+      <name val="Calibri (Body)"/>
+    </font>
   </fonts>
   <fills count="17">
     <fill>
@@ -1217,7 +1261,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="15">
+  <borders count="16">
     <border>
       <left/>
       <right/>
@@ -1425,12 +1469,25 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="74">
+  <cellXfs count="78">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1600,14 +1657,9 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="15" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="15" borderId="0" xfId="1" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="16" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -1621,6 +1673,23 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="15" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="15" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="15" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1837,15 +1906,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:DO995"/>
+  <dimension ref="A1:DO998"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C33" sqref="C33"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="167" workbookViewId="0">
+      <selection activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="2" width="21.5" customWidth="1"/>
+    <col min="1" max="1" width="28.83203125" customWidth="1"/>
+    <col min="2" max="2" width="21.5" customWidth="1"/>
     <col min="3" max="3" width="31.1640625" customWidth="1"/>
     <col min="4" max="8" width="21.5" customWidth="1"/>
     <col min="9" max="9" width="10.5" customWidth="1"/>
@@ -1858,7 +1928,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="63" t="s">
-        <v>307</v>
+        <v>303</v>
       </c>
       <c r="C1" s="63" t="s">
         <v>1</v>
@@ -1914,7 +1984,7 @@
       <c r="E2" s="64" t="s">
         <v>9</v>
       </c>
-      <c r="F2" s="65" t="s">
+      <c r="F2" t="s">
         <v>242</v>
       </c>
       <c r="G2" s="64" t="s">
@@ -1943,7 +2013,7 @@
     </row>
     <row r="3" spans="1:119" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="64" t="s">
-        <v>244</v>
+        <v>318</v>
       </c>
       <c r="B3" s="64"/>
       <c r="C3" s="64" t="s">
@@ -1953,10 +2023,10 @@
         <v>8</v>
       </c>
       <c r="E3" s="64" t="s">
-        <v>9</v>
-      </c>
-      <c r="F3" s="64" t="s">
-        <v>245</v>
+        <v>12</v>
+      </c>
+      <c r="F3" t="s">
+        <v>242</v>
       </c>
       <c r="G3" s="64" t="s">
         <v>246</v>
@@ -1984,7 +2054,7 @@
     </row>
     <row r="4" spans="1:119" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="64" t="s">
-        <v>247</v>
+        <v>249</v>
       </c>
       <c r="B4" s="64"/>
       <c r="C4" s="64" t="s">
@@ -1997,10 +2067,10 @@
         <v>9</v>
       </c>
       <c r="F4" t="s">
-        <v>248</v>
+        <v>313</v>
       </c>
       <c r="G4" s="64" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="H4" s="64">
         <v>401</v>
@@ -2025,7 +2095,7 @@
     </row>
     <row r="5" spans="1:119" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="64" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="B5" s="64"/>
       <c r="C5" s="64" t="s">
@@ -2038,10 +2108,10 @@
         <v>9</v>
       </c>
       <c r="F5" s="64" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="G5" s="64" t="s">
-        <v>246</v>
+        <v>250</v>
       </c>
       <c r="H5" s="64">
         <v>401</v>
@@ -2066,7 +2136,7 @@
     </row>
     <row r="6" spans="1:119" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="64" t="s">
-        <v>252</v>
+        <v>308</v>
       </c>
       <c r="B6" s="64"/>
       <c r="C6" s="64" t="s">
@@ -2078,15 +2148,11 @@
       <c r="E6" s="64" t="s">
         <v>9</v>
       </c>
-      <c r="F6" s="64" t="s">
-        <v>253</v>
-      </c>
-      <c r="G6" s="64" t="s">
-        <v>251</v>
-      </c>
-      <c r="H6" s="64">
-        <v>401</v>
-      </c>
+      <c r="F6" t="s">
+        <v>314</v>
+      </c>
+      <c r="G6" s="64"/>
+      <c r="H6" s="64"/>
       <c r="I6" s="64"/>
       <c r="J6" s="1"/>
       <c r="K6" s="1"/>
@@ -2107,7 +2173,7 @@
     </row>
     <row r="7" spans="1:119" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="64" t="s">
-        <v>254</v>
+        <v>319</v>
       </c>
       <c r="B7" s="64"/>
       <c r="C7" s="64" t="s">
@@ -2119,9 +2185,11 @@
       <c r="E7" s="64" t="s">
         <v>9</v>
       </c>
-      <c r="F7" s="64"/>
+      <c r="F7" t="s">
+        <v>247</v>
+      </c>
       <c r="G7" s="64" t="s">
-        <v>246</v>
+        <v>248</v>
       </c>
       <c r="H7" s="64">
         <v>401</v>
@@ -2146,7 +2214,7 @@
     </row>
     <row r="8" spans="1:119" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="64" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="B8" s="64"/>
       <c r="C8" s="64" t="s">
@@ -2183,7 +2251,7 @@
     </row>
     <row r="9" spans="1:119" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="64" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="B9" s="64"/>
       <c r="C9" s="64" t="s">
@@ -2196,9 +2264,11 @@
         <v>9</v>
       </c>
       <c r="F9" s="64"/>
-      <c r="G9" s="64"/>
+      <c r="G9" s="64" t="s">
+        <v>246</v>
+      </c>
       <c r="H9" s="64">
-        <v>400</v>
+        <v>401</v>
       </c>
       <c r="I9" s="64"/>
       <c r="J9" s="1"/>
@@ -2220,7 +2290,7 @@
     </row>
     <row r="10" spans="1:119" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="64" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="B10" s="64"/>
       <c r="C10" s="64" t="s">
@@ -2232,14 +2302,10 @@
       <c r="E10" s="64" t="s">
         <v>9</v>
       </c>
-      <c r="F10" s="65" t="s">
-        <v>248</v>
-      </c>
-      <c r="G10" s="64" t="s">
-        <v>246</v>
-      </c>
+      <c r="F10" s="64"/>
+      <c r="G10" s="64"/>
       <c r="H10" s="64">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="I10" s="64"/>
       <c r="J10" s="1"/>
@@ -2261,11 +2327,11 @@
     </row>
     <row r="11" spans="1:119" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="64" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="B11" s="64"/>
       <c r="C11" s="64" t="s">
-        <v>10</v>
+        <v>312</v>
       </c>
       <c r="D11" s="64" t="s">
         <v>8</v>
@@ -2273,14 +2339,14 @@
       <c r="E11" s="64" t="s">
         <v>9</v>
       </c>
-      <c r="F11" s="65" t="s">
-        <v>248</v>
+      <c r="F11" t="s">
+        <v>247</v>
       </c>
       <c r="G11" s="64" t="s">
         <v>246</v>
       </c>
       <c r="H11" s="64">
-        <v>400</v>
+        <v>401</v>
       </c>
       <c r="I11" s="64"/>
       <c r="J11" s="1"/>
@@ -2302,26 +2368,26 @@
     </row>
     <row r="12" spans="1:119" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="64" t="s">
-        <v>259</v>
+        <v>311</v>
       </c>
       <c r="B12" s="64"/>
       <c r="C12" s="64" t="s">
         <v>10</v>
       </c>
       <c r="D12" s="64" t="s">
-        <v>260</v>
+        <v>8</v>
       </c>
       <c r="E12" s="64" t="s">
         <v>9</v>
       </c>
-      <c r="F12" s="65" t="s">
-        <v>248</v>
+      <c r="F12" t="s">
+        <v>247</v>
       </c>
       <c r="G12" s="64" t="s">
         <v>246</v>
       </c>
       <c r="H12" s="64">
-        <v>415</v>
+        <v>400</v>
       </c>
       <c r="I12" s="64"/>
       <c r="J12" s="1"/>
@@ -2341,28 +2407,28 @@
       <c r="X12" s="1"/>
       <c r="Y12" s="1"/>
     </row>
-    <row r="13" spans="1:119" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:119" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="64" t="s">
-        <v>261</v>
+        <v>310</v>
       </c>
       <c r="B13" s="64"/>
       <c r="C13" s="64" t="s">
         <v>10</v>
       </c>
       <c r="D13" s="64" t="s">
-        <v>8</v>
+        <v>257</v>
       </c>
       <c r="E13" s="64" t="s">
-        <v>12</v>
-      </c>
-      <c r="F13" s="65" t="s">
-        <v>248</v>
+        <v>9</v>
+      </c>
+      <c r="F13" t="s">
+        <v>247</v>
       </c>
       <c r="G13" s="64" t="s">
         <v>246</v>
       </c>
       <c r="H13" s="64">
-        <v>405</v>
+        <v>415</v>
       </c>
       <c r="I13" s="64"/>
       <c r="J13" s="1"/>
@@ -2382,26 +2448,28 @@
       <c r="X13" s="1"/>
       <c r="Y13" s="1"/>
     </row>
-    <row r="14" spans="1:119" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:119" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="64" t="s">
-        <v>262</v>
+        <v>320</v>
       </c>
       <c r="B14" s="64"/>
       <c r="C14" s="64" t="s">
-        <v>263</v>
+        <v>10</v>
       </c>
       <c r="D14" s="64" t="s">
         <v>8</v>
       </c>
       <c r="E14" s="64" t="s">
-        <v>9</v>
-      </c>
-      <c r="F14" s="66" t="s">
-        <v>248</v>
-      </c>
-      <c r="G14" s="64"/>
+        <v>12</v>
+      </c>
+      <c r="F14" t="s">
+        <v>247</v>
+      </c>
+      <c r="G14" s="64" t="s">
+        <v>246</v>
+      </c>
       <c r="H14" s="64">
-        <v>201</v>
+        <v>405</v>
       </c>
       <c r="I14" s="64"/>
       <c r="J14" s="1"/>
@@ -2420,123 +2488,29 @@
       <c r="W14" s="1"/>
       <c r="X14" s="1"/>
       <c r="Y14" s="1"/>
-      <c r="Z14" s="1"/>
-      <c r="AA14" s="1"/>
-      <c r="AB14" s="1"/>
-      <c r="AC14" s="1"/>
-      <c r="AD14" s="1"/>
-      <c r="AE14" s="1"/>
-      <c r="AF14" s="1"/>
-      <c r="AG14" s="1"/>
-      <c r="AH14" s="1"/>
-      <c r="AI14" s="1"/>
-      <c r="AJ14" s="1"/>
-      <c r="AK14" s="1"/>
-      <c r="AL14" s="1"/>
-      <c r="AM14" s="1"/>
-      <c r="AN14" s="1"/>
-      <c r="AO14" s="1"/>
-      <c r="AP14" s="1"/>
-      <c r="AQ14" s="1"/>
-      <c r="AR14" s="1"/>
-      <c r="AS14" s="1"/>
-      <c r="AT14" s="1"/>
-      <c r="AU14" s="1"/>
-      <c r="AV14" s="1"/>
-      <c r="AW14" s="1"/>
-      <c r="AX14" s="1"/>
-      <c r="AY14" s="1"/>
-      <c r="AZ14" s="1"/>
-      <c r="BA14" s="1"/>
-      <c r="BB14" s="1"/>
-      <c r="BC14" s="1"/>
-      <c r="BD14" s="1"/>
-      <c r="BE14" s="1"/>
-      <c r="BF14" s="1"/>
-      <c r="BG14" s="1"/>
-      <c r="BH14" s="1"/>
-      <c r="BI14" s="1"/>
-      <c r="BJ14" s="1"/>
-      <c r="BK14" s="1"/>
-      <c r="BL14" s="1"/>
-      <c r="BM14" s="1"/>
-      <c r="BN14" s="1"/>
-      <c r="BO14" s="1"/>
-      <c r="BP14" s="1"/>
-      <c r="BQ14" s="1"/>
-      <c r="BR14" s="1"/>
-      <c r="BS14" s="1"/>
-      <c r="BT14" s="1"/>
-      <c r="BU14" s="1"/>
-      <c r="BV14" s="1"/>
-      <c r="BW14" s="1"/>
-      <c r="BX14" s="1"/>
-      <c r="BY14" s="1"/>
-      <c r="BZ14" s="1"/>
-      <c r="CA14" s="1"/>
-      <c r="CB14" s="1"/>
-      <c r="CC14" s="1"/>
-      <c r="CD14" s="1"/>
-      <c r="CE14" s="1"/>
-      <c r="CF14" s="1"/>
-      <c r="CG14" s="1"/>
-      <c r="CH14" s="1"/>
-      <c r="CI14" s="1"/>
-      <c r="CJ14" s="1"/>
-      <c r="CK14" s="1"/>
-      <c r="CL14" s="1"/>
-      <c r="CM14" s="1"/>
-      <c r="CN14" s="1"/>
-      <c r="CO14" s="1"/>
-      <c r="CP14" s="1"/>
-      <c r="CQ14" s="1"/>
-      <c r="CR14" s="1"/>
-      <c r="CS14" s="1"/>
-      <c r="CT14" s="1"/>
-      <c r="CU14" s="1"/>
-      <c r="CV14" s="1"/>
-      <c r="CW14" s="1"/>
-      <c r="CX14" s="1"/>
-      <c r="CY14" s="1"/>
-      <c r="CZ14" s="1"/>
-      <c r="DA14" s="1"/>
-      <c r="DB14" s="1"/>
-      <c r="DC14" s="1"/>
-      <c r="DD14" s="1"/>
-      <c r="DE14" s="1"/>
-      <c r="DF14" s="1"/>
-      <c r="DG14" s="1"/>
-      <c r="DH14" s="1"/>
-      <c r="DI14" s="1"/>
-      <c r="DJ14" s="1"/>
-      <c r="DK14" s="1"/>
-      <c r="DL14" s="1"/>
-      <c r="DM14" s="1"/>
-      <c r="DN14" s="1"/>
-      <c r="DO14" s="1"/>
     </row>
     <row r="15" spans="1:119" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="64" t="s">
-        <v>244</v>
-      </c>
-      <c r="B15" s="64"/>
-      <c r="C15" s="64" t="s">
-        <v>263</v>
-      </c>
-      <c r="D15" s="64" t="s">
+      <c r="A15" s="71" t="s">
+        <v>258</v>
+      </c>
+      <c r="B15" s="71"/>
+      <c r="C15" s="71" t="s">
+        <v>259</v>
+      </c>
+      <c r="D15" s="71" t="s">
         <v>8</v>
       </c>
-      <c r="E15" s="64" t="s">
+      <c r="E15" s="71" t="s">
         <v>9</v>
       </c>
-      <c r="F15" s="64" t="s">
-        <v>245</v>
-      </c>
-      <c r="G15" s="64"/>
-      <c r="H15" s="64">
-        <v>401</v>
-      </c>
-      <c r="I15" s="64"/>
+      <c r="F15" s="72" t="s">
+        <v>247</v>
+      </c>
+      <c r="G15" s="71"/>
+      <c r="H15" s="71">
+        <v>201</v>
+      </c>
+      <c r="I15" s="71"/>
       <c r="J15" s="1"/>
       <c r="K15" s="1"/>
       <c r="L15" s="1"/>
@@ -2553,29 +2527,123 @@
       <c r="W15" s="1"/>
       <c r="X15" s="1"/>
       <c r="Y15" s="1"/>
+      <c r="Z15" s="1"/>
+      <c r="AA15" s="1"/>
+      <c r="AB15" s="1"/>
+      <c r="AC15" s="1"/>
+      <c r="AD15" s="1"/>
+      <c r="AE15" s="1"/>
+      <c r="AF15" s="1"/>
+      <c r="AG15" s="1"/>
+      <c r="AH15" s="1"/>
+      <c r="AI15" s="1"/>
+      <c r="AJ15" s="1"/>
+      <c r="AK15" s="1"/>
+      <c r="AL15" s="1"/>
+      <c r="AM15" s="1"/>
+      <c r="AN15" s="1"/>
+      <c r="AO15" s="1"/>
+      <c r="AP15" s="1"/>
+      <c r="AQ15" s="1"/>
+      <c r="AR15" s="1"/>
+      <c r="AS15" s="1"/>
+      <c r="AT15" s="1"/>
+      <c r="AU15" s="1"/>
+      <c r="AV15" s="1"/>
+      <c r="AW15" s="1"/>
+      <c r="AX15" s="1"/>
+      <c r="AY15" s="1"/>
+      <c r="AZ15" s="1"/>
+      <c r="BA15" s="1"/>
+      <c r="BB15" s="1"/>
+      <c r="BC15" s="1"/>
+      <c r="BD15" s="1"/>
+      <c r="BE15" s="1"/>
+      <c r="BF15" s="1"/>
+      <c r="BG15" s="1"/>
+      <c r="BH15" s="1"/>
+      <c r="BI15" s="1"/>
+      <c r="BJ15" s="1"/>
+      <c r="BK15" s="1"/>
+      <c r="BL15" s="1"/>
+      <c r="BM15" s="1"/>
+      <c r="BN15" s="1"/>
+      <c r="BO15" s="1"/>
+      <c r="BP15" s="1"/>
+      <c r="BQ15" s="1"/>
+      <c r="BR15" s="1"/>
+      <c r="BS15" s="1"/>
+      <c r="BT15" s="1"/>
+      <c r="BU15" s="1"/>
+      <c r="BV15" s="1"/>
+      <c r="BW15" s="1"/>
+      <c r="BX15" s="1"/>
+      <c r="BY15" s="1"/>
+      <c r="BZ15" s="1"/>
+      <c r="CA15" s="1"/>
+      <c r="CB15" s="1"/>
+      <c r="CC15" s="1"/>
+      <c r="CD15" s="1"/>
+      <c r="CE15" s="1"/>
+      <c r="CF15" s="1"/>
+      <c r="CG15" s="1"/>
+      <c r="CH15" s="1"/>
+      <c r="CI15" s="1"/>
+      <c r="CJ15" s="1"/>
+      <c r="CK15" s="1"/>
+      <c r="CL15" s="1"/>
+      <c r="CM15" s="1"/>
+      <c r="CN15" s="1"/>
+      <c r="CO15" s="1"/>
+      <c r="CP15" s="1"/>
+      <c r="CQ15" s="1"/>
+      <c r="CR15" s="1"/>
+      <c r="CS15" s="1"/>
+      <c r="CT15" s="1"/>
+      <c r="CU15" s="1"/>
+      <c r="CV15" s="1"/>
+      <c r="CW15" s="1"/>
+      <c r="CX15" s="1"/>
+      <c r="CY15" s="1"/>
+      <c r="CZ15" s="1"/>
+      <c r="DA15" s="1"/>
+      <c r="DB15" s="1"/>
+      <c r="DC15" s="1"/>
+      <c r="DD15" s="1"/>
+      <c r="DE15" s="1"/>
+      <c r="DF15" s="1"/>
+      <c r="DG15" s="1"/>
+      <c r="DH15" s="1"/>
+      <c r="DI15" s="1"/>
+      <c r="DJ15" s="1"/>
+      <c r="DK15" s="1"/>
+      <c r="DL15" s="1"/>
+      <c r="DM15" s="1"/>
+      <c r="DN15" s="1"/>
+      <c r="DO15" s="1"/>
     </row>
     <row r="16" spans="1:119" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="64" t="s">
-        <v>256</v>
-      </c>
-      <c r="B16" s="64"/>
-      <c r="C16" s="64" t="s">
-        <v>263</v>
-      </c>
-      <c r="D16" s="64" t="s">
+      <c r="A16" s="71" t="s">
+        <v>323</v>
+      </c>
+      <c r="B16" s="71"/>
+      <c r="C16" s="71" t="s">
+        <v>259</v>
+      </c>
+      <c r="D16" s="71" t="s">
         <v>8</v>
       </c>
-      <c r="E16" s="64" t="s">
+      <c r="E16" s="71" t="s">
         <v>9</v>
       </c>
-      <c r="F16" s="64" t="s">
-        <v>27</v>
-      </c>
-      <c r="G16" s="64"/>
-      <c r="H16" s="64">
-        <v>401</v>
-      </c>
-      <c r="I16" s="64"/>
+      <c r="F16" s="72" t="s">
+        <v>313</v>
+      </c>
+      <c r="G16" s="71"/>
+      <c r="H16" s="71">
+        <v>400</v>
+      </c>
+      <c r="I16" s="71"/>
       <c r="J16" s="1"/>
       <c r="K16" s="1"/>
       <c r="L16" s="1"/>
@@ -2592,29 +2660,123 @@
       <c r="W16" s="1"/>
       <c r="X16" s="1"/>
       <c r="Y16" s="1"/>
+      <c r="Z16" s="1"/>
+      <c r="AA16" s="1"/>
+      <c r="AB16" s="1"/>
+      <c r="AC16" s="1"/>
+      <c r="AD16" s="1"/>
+      <c r="AE16" s="1"/>
+      <c r="AF16" s="1"/>
+      <c r="AG16" s="1"/>
+      <c r="AH16" s="1"/>
+      <c r="AI16" s="1"/>
+      <c r="AJ16" s="1"/>
+      <c r="AK16" s="1"/>
+      <c r="AL16" s="1"/>
+      <c r="AM16" s="1"/>
+      <c r="AN16" s="1"/>
+      <c r="AO16" s="1"/>
+      <c r="AP16" s="1"/>
+      <c r="AQ16" s="1"/>
+      <c r="AR16" s="1"/>
+      <c r="AS16" s="1"/>
+      <c r="AT16" s="1"/>
+      <c r="AU16" s="1"/>
+      <c r="AV16" s="1"/>
+      <c r="AW16" s="1"/>
+      <c r="AX16" s="1"/>
+      <c r="AY16" s="1"/>
+      <c r="AZ16" s="1"/>
+      <c r="BA16" s="1"/>
+      <c r="BB16" s="1"/>
+      <c r="BC16" s="1"/>
+      <c r="BD16" s="1"/>
+      <c r="BE16" s="1"/>
+      <c r="BF16" s="1"/>
+      <c r="BG16" s="1"/>
+      <c r="BH16" s="1"/>
+      <c r="BI16" s="1"/>
+      <c r="BJ16" s="1"/>
+      <c r="BK16" s="1"/>
+      <c r="BL16" s="1"/>
+      <c r="BM16" s="1"/>
+      <c r="BN16" s="1"/>
+      <c r="BO16" s="1"/>
+      <c r="BP16" s="1"/>
+      <c r="BQ16" s="1"/>
+      <c r="BR16" s="1"/>
+      <c r="BS16" s="1"/>
+      <c r="BT16" s="1"/>
+      <c r="BU16" s="1"/>
+      <c r="BV16" s="1"/>
+      <c r="BW16" s="1"/>
+      <c r="BX16" s="1"/>
+      <c r="BY16" s="1"/>
+      <c r="BZ16" s="1"/>
+      <c r="CA16" s="1"/>
+      <c r="CB16" s="1"/>
+      <c r="CC16" s="1"/>
+      <c r="CD16" s="1"/>
+      <c r="CE16" s="1"/>
+      <c r="CF16" s="1"/>
+      <c r="CG16" s="1"/>
+      <c r="CH16" s="1"/>
+      <c r="CI16" s="1"/>
+      <c r="CJ16" s="1"/>
+      <c r="CK16" s="1"/>
+      <c r="CL16" s="1"/>
+      <c r="CM16" s="1"/>
+      <c r="CN16" s="1"/>
+      <c r="CO16" s="1"/>
+      <c r="CP16" s="1"/>
+      <c r="CQ16" s="1"/>
+      <c r="CR16" s="1"/>
+      <c r="CS16" s="1"/>
+      <c r="CT16" s="1"/>
+      <c r="CU16" s="1"/>
+      <c r="CV16" s="1"/>
+      <c r="CW16" s="1"/>
+      <c r="CX16" s="1"/>
+      <c r="CY16" s="1"/>
+      <c r="CZ16" s="1"/>
+      <c r="DA16" s="1"/>
+      <c r="DB16" s="1"/>
+      <c r="DC16" s="1"/>
+      <c r="DD16" s="1"/>
+      <c r="DE16" s="1"/>
+      <c r="DF16" s="1"/>
+      <c r="DG16" s="1"/>
+      <c r="DH16" s="1"/>
+      <c r="DI16" s="1"/>
+      <c r="DJ16" s="1"/>
+      <c r="DK16" s="1"/>
+      <c r="DL16" s="1"/>
+      <c r="DM16" s="1"/>
+      <c r="DN16" s="1"/>
+      <c r="DO16" s="1"/>
     </row>
     <row r="17" spans="1:119" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="64" t="s">
-        <v>257</v>
-      </c>
-      <c r="B17" s="64"/>
-      <c r="C17" s="64" t="s">
-        <v>263</v>
-      </c>
-      <c r="D17" s="64" t="s">
+      <c r="A17" s="71" t="s">
+        <v>244</v>
+      </c>
+      <c r="B17" s="71"/>
+      <c r="C17" s="71" t="s">
+        <v>259</v>
+      </c>
+      <c r="D17" s="71" t="s">
         <v>8</v>
       </c>
-      <c r="E17" s="64" t="s">
+      <c r="E17" s="71" t="s">
         <v>9</v>
       </c>
-      <c r="F17" s="64" t="s">
-        <v>253</v>
-      </c>
-      <c r="G17" s="64"/>
-      <c r="H17" s="64">
-        <v>404</v>
-      </c>
-      <c r="I17" s="64"/>
+      <c r="F17" s="71" t="s">
+        <v>245</v>
+      </c>
+      <c r="G17" s="71"/>
+      <c r="H17" s="71">
+        <v>401</v>
+      </c>
+      <c r="I17" s="71"/>
       <c r="J17" s="1"/>
       <c r="K17" s="1"/>
       <c r="L17" s="1"/>
@@ -2633,29 +2795,25 @@
       <c r="Y17" s="1"/>
     </row>
     <row r="18" spans="1:119" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="67" t="s">
-        <v>265</v>
-      </c>
-      <c r="B18" s="67"/>
-      <c r="C18" s="67" t="s">
-        <v>266</v>
-      </c>
-      <c r="D18" s="67" t="s">
+      <c r="A18" s="71" t="s">
+        <v>255</v>
+      </c>
+      <c r="B18" s="71"/>
+      <c r="C18" s="71" t="s">
+        <v>259</v>
+      </c>
+      <c r="D18" s="71" t="s">
         <v>8</v>
       </c>
-      <c r="E18" s="67" t="s">
+      <c r="E18" s="71" t="s">
         <v>9</v>
       </c>
-      <c r="F18" s="68" t="s">
-        <v>248</v>
-      </c>
-      <c r="G18" s="67" t="s">
-        <v>267</v>
-      </c>
-      <c r="H18" s="67">
-        <v>200</v>
-      </c>
-      <c r="I18" s="67"/>
+      <c r="F18" s="72"/>
+      <c r="G18" s="71"/>
+      <c r="H18" s="71">
+        <v>401</v>
+      </c>
+      <c r="I18" s="71"/>
       <c r="J18" s="1"/>
       <c r="K18" s="1"/>
       <c r="L18" s="1"/>
@@ -2674,19 +2832,27 @@
       <c r="Y18" s="1"/>
     </row>
     <row r="19" spans="1:119" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="67" t="s">
-        <v>268</v>
-      </c>
-      <c r="B19" s="67"/>
-      <c r="C19" s="67" t="s">
-        <v>266</v>
-      </c>
-      <c r="D19" s="67"/>
-      <c r="E19" s="67"/>
-      <c r="F19" s="68"/>
-      <c r="G19" s="67"/>
-      <c r="H19" s="67"/>
-      <c r="I19" s="67"/>
+      <c r="A19" s="71" t="s">
+        <v>321</v>
+      </c>
+      <c r="B19" s="71"/>
+      <c r="C19" s="71" t="s">
+        <v>259</v>
+      </c>
+      <c r="D19" s="71" t="s">
+        <v>322</v>
+      </c>
+      <c r="E19" s="71" t="s">
+        <v>9</v>
+      </c>
+      <c r="F19" s="72" t="s">
+        <v>247</v>
+      </c>
+      <c r="G19" s="71"/>
+      <c r="H19" s="71">
+        <v>404</v>
+      </c>
+      <c r="I19" s="71"/>
       <c r="J19" s="1"/>
       <c r="K19" s="1"/>
       <c r="L19" s="1"/>
@@ -2705,29 +2871,27 @@
       <c r="Y19" s="1"/>
     </row>
     <row r="20" spans="1:119" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="67" t="s">
+      <c r="A20" s="71" t="s">
+        <v>256</v>
+      </c>
+      <c r="B20" s="71"/>
+      <c r="C20" s="71" t="s">
+        <v>315</v>
+      </c>
+      <c r="D20" s="71" t="s">
+        <v>8</v>
+      </c>
+      <c r="E20" s="71" t="s">
+        <v>9</v>
+      </c>
+      <c r="F20" s="75" t="s">
         <v>252</v>
       </c>
-      <c r="B20" s="67"/>
-      <c r="C20" s="67" t="s">
-        <v>266</v>
-      </c>
-      <c r="D20" s="67" t="s">
-        <v>8</v>
-      </c>
-      <c r="E20" s="67" t="s">
-        <v>9</v>
-      </c>
-      <c r="F20" s="67" t="s">
-        <v>253</v>
-      </c>
-      <c r="G20" s="67" t="s">
-        <v>269</v>
-      </c>
-      <c r="H20" s="67">
-        <v>400</v>
-      </c>
-      <c r="I20" s="67"/>
+      <c r="G20" s="75"/>
+      <c r="H20" s="71">
+        <v>404</v>
+      </c>
+      <c r="I20" s="71"/>
       <c r="J20" s="1"/>
       <c r="K20" s="1"/>
       <c r="L20" s="1"/>
@@ -2746,29 +2910,31 @@
       <c r="Y20" s="1"/>
     </row>
     <row r="21" spans="1:119" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="67" t="s">
-        <v>244</v>
-      </c>
-      <c r="B21" s="67"/>
-      <c r="C21" s="67" t="s">
-        <v>266</v>
-      </c>
-      <c r="D21" s="67" t="s">
+      <c r="A21" s="65" t="s">
+        <v>261</v>
+      </c>
+      <c r="B21" s="65" t="s">
+        <v>316</v>
+      </c>
+      <c r="C21" s="65" t="s">
+        <v>262</v>
+      </c>
+      <c r="D21" s="65" t="s">
         <v>8</v>
       </c>
-      <c r="E21" s="67" t="s">
+      <c r="E21" s="73" t="s">
         <v>9</v>
       </c>
-      <c r="F21" s="67" t="s">
-        <v>245</v>
-      </c>
-      <c r="G21" s="67" t="s">
-        <v>267</v>
-      </c>
-      <c r="H21" s="67">
-        <v>400</v>
-      </c>
-      <c r="I21" s="67"/>
+      <c r="F21" s="3" t="s">
+        <v>247</v>
+      </c>
+      <c r="G21" s="77" t="s">
+        <v>324</v>
+      </c>
+      <c r="H21" s="74">
+        <v>200</v>
+      </c>
+      <c r="I21" s="65"/>
       <c r="J21" s="1"/>
       <c r="K21" s="1"/>
       <c r="L21" s="1"/>
@@ -2787,25 +2953,29 @@
       <c r="Y21" s="1"/>
     </row>
     <row r="22" spans="1:119" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="69" t="s">
-        <v>265</v>
-      </c>
-      <c r="B22" s="69"/>
-      <c r="C22" s="69" t="s">
-        <v>311</v>
-      </c>
-      <c r="D22" s="69" t="s">
+      <c r="A22" s="65" t="s">
+        <v>264</v>
+      </c>
+      <c r="B22" s="65" t="s">
+        <v>317</v>
+      </c>
+      <c r="C22" s="65" t="s">
+        <v>262</v>
+      </c>
+      <c r="D22" s="65" t="s">
         <v>8</v>
       </c>
-      <c r="E22" s="69" t="s">
-        <v>12</v>
-      </c>
-      <c r="F22" s="69"/>
-      <c r="G22" s="69"/>
-      <c r="H22" s="69">
-        <v>200</v>
-      </c>
-      <c r="I22" s="69"/>
+      <c r="E22" s="73" t="s">
+        <v>9</v>
+      </c>
+      <c r="F22" s="3" t="s">
+        <v>247</v>
+      </c>
+      <c r="G22" s="3" t="s">
+        <v>309</v>
+      </c>
+      <c r="H22" s="74"/>
+      <c r="I22" s="65"/>
       <c r="J22" s="1"/>
       <c r="K22" s="1"/>
       <c r="L22" s="1"/>
@@ -2824,25 +2994,31 @@
       <c r="Y22" s="1"/>
     </row>
     <row r="23" spans="1:119" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="69" t="s">
+      <c r="A23" s="65" t="s">
+        <v>251</v>
+      </c>
+      <c r="B23" s="65" t="s">
+        <v>316</v>
+      </c>
+      <c r="C23" s="65" t="s">
+        <v>262</v>
+      </c>
+      <c r="D23" s="65" t="s">
+        <v>8</v>
+      </c>
+      <c r="E23" s="65" t="s">
+        <v>9</v>
+      </c>
+      <c r="F23" s="76" t="s">
         <v>252</v>
       </c>
-      <c r="B23" s="69"/>
-      <c r="C23" s="69" t="s">
-        <v>311</v>
-      </c>
-      <c r="D23" s="69" t="s">
-        <v>8</v>
-      </c>
-      <c r="E23" s="69" t="s">
-        <v>12</v>
-      </c>
-      <c r="F23" s="69"/>
-      <c r="G23" s="69"/>
-      <c r="H23" s="69">
-        <v>401</v>
-      </c>
-      <c r="I23" s="69"/>
+      <c r="G23" s="76" t="s">
+        <v>265</v>
+      </c>
+      <c r="H23" s="65">
+        <v>400</v>
+      </c>
+      <c r="I23" s="65"/>
       <c r="J23" s="1"/>
       <c r="K23" s="1"/>
       <c r="L23" s="1"/>
@@ -2861,25 +3037,31 @@
       <c r="Y23" s="1"/>
     </row>
     <row r="24" spans="1:119" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="69" t="s">
+      <c r="A24" s="65" t="s">
         <v>244</v>
       </c>
-      <c r="B24" s="69"/>
-      <c r="C24" s="69" t="s">
-        <v>311</v>
-      </c>
-      <c r="D24" s="69" t="s">
+      <c r="B24" s="65" t="s">
+        <v>316</v>
+      </c>
+      <c r="C24" s="65" t="s">
+        <v>262</v>
+      </c>
+      <c r="D24" s="65" t="s">
         <v>8</v>
       </c>
-      <c r="E24" s="69" t="s">
-        <v>12</v>
-      </c>
-      <c r="F24" s="72"/>
-      <c r="G24" s="69"/>
-      <c r="H24" s="69">
-        <v>401</v>
-      </c>
-      <c r="I24" s="69"/>
+      <c r="E24" s="65" t="s">
+        <v>9</v>
+      </c>
+      <c r="F24" s="65" t="s">
+        <v>245</v>
+      </c>
+      <c r="G24" s="65" t="s">
+        <v>263</v>
+      </c>
+      <c r="H24" s="65">
+        <v>400</v>
+      </c>
+      <c r="I24" s="65"/>
       <c r="J24" s="1"/>
       <c r="K24" s="1"/>
       <c r="L24" s="1"/>
@@ -2898,25 +3080,29 @@
       <c r="Y24" s="1"/>
     </row>
     <row r="25" spans="1:119" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="64"/>
-      <c r="B25" s="64" t="s">
-        <v>308</v>
-      </c>
-      <c r="C25" s="64" t="s">
-        <v>264</v>
-      </c>
-      <c r="D25" s="64" t="s">
+      <c r="A25" s="66" t="s">
+        <v>261</v>
+      </c>
+      <c r="B25" s="66"/>
+      <c r="C25" s="66" t="s">
+        <v>307</v>
+      </c>
+      <c r="D25" s="66" t="s">
         <v>8</v>
       </c>
-      <c r="E25" s="70" t="s">
+      <c r="E25" s="66" t="s">
         <v>12</v>
       </c>
-      <c r="F25" s="73"/>
-      <c r="G25" s="71"/>
-      <c r="H25" s="64">
+      <c r="F25" s="69" t="s">
+        <v>247</v>
+      </c>
+      <c r="G25" s="69" t="s">
+        <v>309</v>
+      </c>
+      <c r="H25" s="66">
         <v>200</v>
       </c>
-      <c r="I25" s="64"/>
+      <c r="I25" s="66"/>
       <c r="J25" s="1"/>
       <c r="K25" s="1"/>
       <c r="L25" s="1"/>
@@ -2933,121 +3119,31 @@
       <c r="W25" s="1"/>
       <c r="X25" s="1"/>
       <c r="Y25" s="1"/>
-      <c r="Z25" s="1"/>
-      <c r="AA25" s="1"/>
-      <c r="AB25" s="1"/>
-      <c r="AC25" s="1"/>
-      <c r="AD25" s="1"/>
-      <c r="AE25" s="1"/>
-      <c r="AF25" s="1"/>
-      <c r="AG25" s="1"/>
-      <c r="AH25" s="1"/>
-      <c r="AI25" s="1"/>
-      <c r="AJ25" s="1"/>
-      <c r="AK25" s="1"/>
-      <c r="AL25" s="1"/>
-      <c r="AM25" s="1"/>
-      <c r="AN25" s="1"/>
-      <c r="AO25" s="1"/>
-      <c r="AP25" s="1"/>
-      <c r="AQ25" s="1"/>
-      <c r="AR25" s="1"/>
-      <c r="AS25" s="1"/>
-      <c r="AT25" s="1"/>
-      <c r="AU25" s="1"/>
-      <c r="AV25" s="1"/>
-      <c r="AW25" s="1"/>
-      <c r="AX25" s="1"/>
-      <c r="AY25" s="1"/>
-      <c r="AZ25" s="1"/>
-      <c r="BA25" s="1"/>
-      <c r="BB25" s="1"/>
-      <c r="BC25" s="1"/>
-      <c r="BD25" s="1"/>
-      <c r="BE25" s="1"/>
-      <c r="BF25" s="1"/>
-      <c r="BG25" s="1"/>
-      <c r="BH25" s="1"/>
-      <c r="BI25" s="1"/>
-      <c r="BJ25" s="1"/>
-      <c r="BK25" s="1"/>
-      <c r="BL25" s="1"/>
-      <c r="BM25" s="1"/>
-      <c r="BN25" s="1"/>
-      <c r="BO25" s="1"/>
-      <c r="BP25" s="1"/>
-      <c r="BQ25" s="1"/>
-      <c r="BR25" s="1"/>
-      <c r="BS25" s="1"/>
-      <c r="BT25" s="1"/>
-      <c r="BU25" s="1"/>
-      <c r="BV25" s="1"/>
-      <c r="BW25" s="1"/>
-      <c r="BX25" s="1"/>
-      <c r="BY25" s="1"/>
-      <c r="BZ25" s="1"/>
-      <c r="CA25" s="1"/>
-      <c r="CB25" s="1"/>
-      <c r="CC25" s="1"/>
-      <c r="CD25" s="1"/>
-      <c r="CE25" s="1"/>
-      <c r="CF25" s="1"/>
-      <c r="CG25" s="1"/>
-      <c r="CH25" s="1"/>
-      <c r="CI25" s="1"/>
-      <c r="CJ25" s="1"/>
-      <c r="CK25" s="1"/>
-      <c r="CL25" s="1"/>
-      <c r="CM25" s="1"/>
-      <c r="CN25" s="1"/>
-      <c r="CO25" s="1"/>
-      <c r="CP25" s="1"/>
-      <c r="CQ25" s="1"/>
-      <c r="CR25" s="1"/>
-      <c r="CS25" s="1"/>
-      <c r="CT25" s="1"/>
-      <c r="CU25" s="1"/>
-      <c r="CV25" s="1"/>
-      <c r="CW25" s="1"/>
-      <c r="CX25" s="1"/>
-      <c r="CY25" s="1"/>
-      <c r="CZ25" s="1"/>
-      <c r="DA25" s="1"/>
-      <c r="DB25" s="1"/>
-      <c r="DC25" s="1"/>
-      <c r="DD25" s="1"/>
-      <c r="DE25" s="1"/>
-      <c r="DF25" s="1"/>
-      <c r="DG25" s="1"/>
-      <c r="DH25" s="1"/>
-      <c r="DI25" s="1"/>
-      <c r="DJ25" s="1"/>
-      <c r="DK25" s="1"/>
-      <c r="DL25" s="1"/>
-      <c r="DM25" s="1"/>
-      <c r="DN25" s="1"/>
-      <c r="DO25" s="1"/>
     </row>
     <row r="26" spans="1:119" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="64"/>
-      <c r="B26" s="64" t="s">
-        <v>309</v>
-      </c>
-      <c r="C26" s="64" t="s">
-        <v>264</v>
-      </c>
-      <c r="D26" s="64" t="s">
+      <c r="A26" s="66" t="s">
+        <v>251</v>
+      </c>
+      <c r="B26" s="66"/>
+      <c r="C26" s="66" t="s">
+        <v>307</v>
+      </c>
+      <c r="D26" s="66" t="s">
         <v>8</v>
       </c>
-      <c r="E26" s="70" t="s">
+      <c r="E26" s="66" t="s">
         <v>12</v>
       </c>
-      <c r="F26" s="73"/>
-      <c r="G26" s="71"/>
-      <c r="H26" s="64">
+      <c r="F26" s="69" t="s">
+        <v>247</v>
+      </c>
+      <c r="G26" s="69" t="s">
+        <v>250</v>
+      </c>
+      <c r="H26" s="66">
         <v>401</v>
       </c>
-      <c r="I26" s="64"/>
+      <c r="I26" s="66"/>
       <c r="J26" s="1"/>
       <c r="K26" s="1"/>
       <c r="L26" s="1"/>
@@ -3064,121 +3160,31 @@
       <c r="W26" s="1"/>
       <c r="X26" s="1"/>
       <c r="Y26" s="1"/>
-      <c r="Z26" s="1"/>
-      <c r="AA26" s="1"/>
-      <c r="AB26" s="1"/>
-      <c r="AC26" s="1"/>
-      <c r="AD26" s="1"/>
-      <c r="AE26" s="1"/>
-      <c r="AF26" s="1"/>
-      <c r="AG26" s="1"/>
-      <c r="AH26" s="1"/>
-      <c r="AI26" s="1"/>
-      <c r="AJ26" s="1"/>
-      <c r="AK26" s="1"/>
-      <c r="AL26" s="1"/>
-      <c r="AM26" s="1"/>
-      <c r="AN26" s="1"/>
-      <c r="AO26" s="1"/>
-      <c r="AP26" s="1"/>
-      <c r="AQ26" s="1"/>
-      <c r="AR26" s="1"/>
-      <c r="AS26" s="1"/>
-      <c r="AT26" s="1"/>
-      <c r="AU26" s="1"/>
-      <c r="AV26" s="1"/>
-      <c r="AW26" s="1"/>
-      <c r="AX26" s="1"/>
-      <c r="AY26" s="1"/>
-      <c r="AZ26" s="1"/>
-      <c r="BA26" s="1"/>
-      <c r="BB26" s="1"/>
-      <c r="BC26" s="1"/>
-      <c r="BD26" s="1"/>
-      <c r="BE26" s="1"/>
-      <c r="BF26" s="1"/>
-      <c r="BG26" s="1"/>
-      <c r="BH26" s="1"/>
-      <c r="BI26" s="1"/>
-      <c r="BJ26" s="1"/>
-      <c r="BK26" s="1"/>
-      <c r="BL26" s="1"/>
-      <c r="BM26" s="1"/>
-      <c r="BN26" s="1"/>
-      <c r="BO26" s="1"/>
-      <c r="BP26" s="1"/>
-      <c r="BQ26" s="1"/>
-      <c r="BR26" s="1"/>
-      <c r="BS26" s="1"/>
-      <c r="BT26" s="1"/>
-      <c r="BU26" s="1"/>
-      <c r="BV26" s="1"/>
-      <c r="BW26" s="1"/>
-      <c r="BX26" s="1"/>
-      <c r="BY26" s="1"/>
-      <c r="BZ26" s="1"/>
-      <c r="CA26" s="1"/>
-      <c r="CB26" s="1"/>
-      <c r="CC26" s="1"/>
-      <c r="CD26" s="1"/>
-      <c r="CE26" s="1"/>
-      <c r="CF26" s="1"/>
-      <c r="CG26" s="1"/>
-      <c r="CH26" s="1"/>
-      <c r="CI26" s="1"/>
-      <c r="CJ26" s="1"/>
-      <c r="CK26" s="1"/>
-      <c r="CL26" s="1"/>
-      <c r="CM26" s="1"/>
-      <c r="CN26" s="1"/>
-      <c r="CO26" s="1"/>
-      <c r="CP26" s="1"/>
-      <c r="CQ26" s="1"/>
-      <c r="CR26" s="1"/>
-      <c r="CS26" s="1"/>
-      <c r="CT26" s="1"/>
-      <c r="CU26" s="1"/>
-      <c r="CV26" s="1"/>
-      <c r="CW26" s="1"/>
-      <c r="CX26" s="1"/>
-      <c r="CY26" s="1"/>
-      <c r="CZ26" s="1"/>
-      <c r="DA26" s="1"/>
-      <c r="DB26" s="1"/>
-      <c r="DC26" s="1"/>
-      <c r="DD26" s="1"/>
-      <c r="DE26" s="1"/>
-      <c r="DF26" s="1"/>
-      <c r="DG26" s="1"/>
-      <c r="DH26" s="1"/>
-      <c r="DI26" s="1"/>
-      <c r="DJ26" s="1"/>
-      <c r="DK26" s="1"/>
-      <c r="DL26" s="1"/>
-      <c r="DM26" s="1"/>
-      <c r="DN26" s="1"/>
-      <c r="DO26" s="1"/>
     </row>
     <row r="27" spans="1:119" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="64"/>
-      <c r="B27" s="64" t="s">
-        <v>310</v>
-      </c>
-      <c r="C27" s="64" t="s">
-        <v>264</v>
-      </c>
-      <c r="D27" s="64" t="s">
+      <c r="A27" s="66" t="s">
+        <v>244</v>
+      </c>
+      <c r="B27" s="66"/>
+      <c r="C27" s="66" t="s">
+        <v>307</v>
+      </c>
+      <c r="D27" s="66" t="s">
         <v>8</v>
       </c>
-      <c r="E27" s="70" t="s">
+      <c r="E27" s="66" t="s">
         <v>12</v>
       </c>
-      <c r="F27" s="73"/>
-      <c r="G27" s="71"/>
-      <c r="H27" s="64">
+      <c r="F27" s="65" t="s">
+        <v>245</v>
+      </c>
+      <c r="G27" s="69" t="s">
+        <v>309</v>
+      </c>
+      <c r="H27" s="66">
         <v>401</v>
       </c>
-      <c r="I27" s="64"/>
+      <c r="I27" s="66"/>
       <c r="J27" s="1"/>
       <c r="K27" s="1"/>
       <c r="L27" s="1"/>
@@ -3195,111 +3201,27 @@
       <c r="W27" s="1"/>
       <c r="X27" s="1"/>
       <c r="Y27" s="1"/>
-      <c r="Z27" s="1"/>
-      <c r="AA27" s="1"/>
-      <c r="AB27" s="1"/>
-      <c r="AC27" s="1"/>
-      <c r="AD27" s="1"/>
-      <c r="AE27" s="1"/>
-      <c r="AF27" s="1"/>
-      <c r="AG27" s="1"/>
-      <c r="AH27" s="1"/>
-      <c r="AI27" s="1"/>
-      <c r="AJ27" s="1"/>
-      <c r="AK27" s="1"/>
-      <c r="AL27" s="1"/>
-      <c r="AM27" s="1"/>
-      <c r="AN27" s="1"/>
-      <c r="AO27" s="1"/>
-      <c r="AP27" s="1"/>
-      <c r="AQ27" s="1"/>
-      <c r="AR27" s="1"/>
-      <c r="AS27" s="1"/>
-      <c r="AT27" s="1"/>
-      <c r="AU27" s="1"/>
-      <c r="AV27" s="1"/>
-      <c r="AW27" s="1"/>
-      <c r="AX27" s="1"/>
-      <c r="AY27" s="1"/>
-      <c r="AZ27" s="1"/>
-      <c r="BA27" s="1"/>
-      <c r="BB27" s="1"/>
-      <c r="BC27" s="1"/>
-      <c r="BD27" s="1"/>
-      <c r="BE27" s="1"/>
-      <c r="BF27" s="1"/>
-      <c r="BG27" s="1"/>
-      <c r="BH27" s="1"/>
-      <c r="BI27" s="1"/>
-      <c r="BJ27" s="1"/>
-      <c r="BK27" s="1"/>
-      <c r="BL27" s="1"/>
-      <c r="BM27" s="1"/>
-      <c r="BN27" s="1"/>
-      <c r="BO27" s="1"/>
-      <c r="BP27" s="1"/>
-      <c r="BQ27" s="1"/>
-      <c r="BR27" s="1"/>
-      <c r="BS27" s="1"/>
-      <c r="BT27" s="1"/>
-      <c r="BU27" s="1"/>
-      <c r="BV27" s="1"/>
-      <c r="BW27" s="1"/>
-      <c r="BX27" s="1"/>
-      <c r="BY27" s="1"/>
-      <c r="BZ27" s="1"/>
-      <c r="CA27" s="1"/>
-      <c r="CB27" s="1"/>
-      <c r="CC27" s="1"/>
-      <c r="CD27" s="1"/>
-      <c r="CE27" s="1"/>
-      <c r="CF27" s="1"/>
-      <c r="CG27" s="1"/>
-      <c r="CH27" s="1"/>
-      <c r="CI27" s="1"/>
-      <c r="CJ27" s="1"/>
-      <c r="CK27" s="1"/>
-      <c r="CL27" s="1"/>
-      <c r="CM27" s="1"/>
-      <c r="CN27" s="1"/>
-      <c r="CO27" s="1"/>
-      <c r="CP27" s="1"/>
-      <c r="CQ27" s="1"/>
-      <c r="CR27" s="1"/>
-      <c r="CS27" s="1"/>
-      <c r="CT27" s="1"/>
-      <c r="CU27" s="1"/>
-      <c r="CV27" s="1"/>
-      <c r="CW27" s="1"/>
-      <c r="CX27" s="1"/>
-      <c r="CY27" s="1"/>
-      <c r="CZ27" s="1"/>
-      <c r="DA27" s="1"/>
-      <c r="DB27" s="1"/>
-      <c r="DC27" s="1"/>
-      <c r="DD27" s="1"/>
-      <c r="DE27" s="1"/>
-      <c r="DF27" s="1"/>
-      <c r="DG27" s="1"/>
-      <c r="DH27" s="1"/>
-      <c r="DI27" s="1"/>
-      <c r="DJ27" s="1"/>
-      <c r="DK27" s="1"/>
-      <c r="DL27" s="1"/>
-      <c r="DM27" s="1"/>
-      <c r="DN27" s="1"/>
-      <c r="DO27" s="1"/>
     </row>
     <row r="28" spans="1:119" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="1"/>
-      <c r="B28" s="1"/>
-      <c r="C28" s="1"/>
-      <c r="D28" s="1"/>
-      <c r="E28" s="1"/>
-      <c r="F28" s="1"/>
-      <c r="G28" s="1"/>
-      <c r="H28" s="1"/>
-      <c r="I28" s="1"/>
+      <c r="A28" s="64"/>
+      <c r="B28" s="64" t="s">
+        <v>304</v>
+      </c>
+      <c r="C28" s="64" t="s">
+        <v>260</v>
+      </c>
+      <c r="D28" s="64" t="s">
+        <v>8</v>
+      </c>
+      <c r="E28" s="67" t="s">
+        <v>12</v>
+      </c>
+      <c r="F28" s="70"/>
+      <c r="G28" s="68"/>
+      <c r="H28" s="64">
+        <v>200</v>
+      </c>
+      <c r="I28" s="64"/>
       <c r="J28" s="1"/>
       <c r="K28" s="1"/>
       <c r="L28" s="1"/>
@@ -3316,17 +3238,121 @@
       <c r="W28" s="1"/>
       <c r="X28" s="1"/>
       <c r="Y28" s="1"/>
+      <c r="Z28" s="1"/>
+      <c r="AA28" s="1"/>
+      <c r="AB28" s="1"/>
+      <c r="AC28" s="1"/>
+      <c r="AD28" s="1"/>
+      <c r="AE28" s="1"/>
+      <c r="AF28" s="1"/>
+      <c r="AG28" s="1"/>
+      <c r="AH28" s="1"/>
+      <c r="AI28" s="1"/>
+      <c r="AJ28" s="1"/>
+      <c r="AK28" s="1"/>
+      <c r="AL28" s="1"/>
+      <c r="AM28" s="1"/>
+      <c r="AN28" s="1"/>
+      <c r="AO28" s="1"/>
+      <c r="AP28" s="1"/>
+      <c r="AQ28" s="1"/>
+      <c r="AR28" s="1"/>
+      <c r="AS28" s="1"/>
+      <c r="AT28" s="1"/>
+      <c r="AU28" s="1"/>
+      <c r="AV28" s="1"/>
+      <c r="AW28" s="1"/>
+      <c r="AX28" s="1"/>
+      <c r="AY28" s="1"/>
+      <c r="AZ28" s="1"/>
+      <c r="BA28" s="1"/>
+      <c r="BB28" s="1"/>
+      <c r="BC28" s="1"/>
+      <c r="BD28" s="1"/>
+      <c r="BE28" s="1"/>
+      <c r="BF28" s="1"/>
+      <c r="BG28" s="1"/>
+      <c r="BH28" s="1"/>
+      <c r="BI28" s="1"/>
+      <c r="BJ28" s="1"/>
+      <c r="BK28" s="1"/>
+      <c r="BL28" s="1"/>
+      <c r="BM28" s="1"/>
+      <c r="BN28" s="1"/>
+      <c r="BO28" s="1"/>
+      <c r="BP28" s="1"/>
+      <c r="BQ28" s="1"/>
+      <c r="BR28" s="1"/>
+      <c r="BS28" s="1"/>
+      <c r="BT28" s="1"/>
+      <c r="BU28" s="1"/>
+      <c r="BV28" s="1"/>
+      <c r="BW28" s="1"/>
+      <c r="BX28" s="1"/>
+      <c r="BY28" s="1"/>
+      <c r="BZ28" s="1"/>
+      <c r="CA28" s="1"/>
+      <c r="CB28" s="1"/>
+      <c r="CC28" s="1"/>
+      <c r="CD28" s="1"/>
+      <c r="CE28" s="1"/>
+      <c r="CF28" s="1"/>
+      <c r="CG28" s="1"/>
+      <c r="CH28" s="1"/>
+      <c r="CI28" s="1"/>
+      <c r="CJ28" s="1"/>
+      <c r="CK28" s="1"/>
+      <c r="CL28" s="1"/>
+      <c r="CM28" s="1"/>
+      <c r="CN28" s="1"/>
+      <c r="CO28" s="1"/>
+      <c r="CP28" s="1"/>
+      <c r="CQ28" s="1"/>
+      <c r="CR28" s="1"/>
+      <c r="CS28" s="1"/>
+      <c r="CT28" s="1"/>
+      <c r="CU28" s="1"/>
+      <c r="CV28" s="1"/>
+      <c r="CW28" s="1"/>
+      <c r="CX28" s="1"/>
+      <c r="CY28" s="1"/>
+      <c r="CZ28" s="1"/>
+      <c r="DA28" s="1"/>
+      <c r="DB28" s="1"/>
+      <c r="DC28" s="1"/>
+      <c r="DD28" s="1"/>
+      <c r="DE28" s="1"/>
+      <c r="DF28" s="1"/>
+      <c r="DG28" s="1"/>
+      <c r="DH28" s="1"/>
+      <c r="DI28" s="1"/>
+      <c r="DJ28" s="1"/>
+      <c r="DK28" s="1"/>
+      <c r="DL28" s="1"/>
+      <c r="DM28" s="1"/>
+      <c r="DN28" s="1"/>
+      <c r="DO28" s="1"/>
     </row>
     <row r="29" spans="1:119" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="1"/>
-      <c r="B29" s="1"/>
-      <c r="C29" s="1"/>
-      <c r="D29" s="1"/>
-      <c r="E29" s="1"/>
-      <c r="F29" s="1"/>
-      <c r="G29" s="1"/>
-      <c r="H29" s="1"/>
-      <c r="I29" s="1"/>
+      <c r="A29" s="64"/>
+      <c r="B29" s="64" t="s">
+        <v>305</v>
+      </c>
+      <c r="C29" s="64" t="s">
+        <v>260</v>
+      </c>
+      <c r="D29" s="64" t="s">
+        <v>8</v>
+      </c>
+      <c r="E29" s="67" t="s">
+        <v>12</v>
+      </c>
+      <c r="F29" s="70"/>
+      <c r="G29" s="68"/>
+      <c r="H29" s="64">
+        <v>401</v>
+      </c>
+      <c r="I29" s="64"/>
       <c r="J29" s="1"/>
       <c r="K29" s="1"/>
       <c r="L29" s="1"/>
@@ -3343,17 +3369,121 @@
       <c r="W29" s="1"/>
       <c r="X29" s="1"/>
       <c r="Y29" s="1"/>
+      <c r="Z29" s="1"/>
+      <c r="AA29" s="1"/>
+      <c r="AB29" s="1"/>
+      <c r="AC29" s="1"/>
+      <c r="AD29" s="1"/>
+      <c r="AE29" s="1"/>
+      <c r="AF29" s="1"/>
+      <c r="AG29" s="1"/>
+      <c r="AH29" s="1"/>
+      <c r="AI29" s="1"/>
+      <c r="AJ29" s="1"/>
+      <c r="AK29" s="1"/>
+      <c r="AL29" s="1"/>
+      <c r="AM29" s="1"/>
+      <c r="AN29" s="1"/>
+      <c r="AO29" s="1"/>
+      <c r="AP29" s="1"/>
+      <c r="AQ29" s="1"/>
+      <c r="AR29" s="1"/>
+      <c r="AS29" s="1"/>
+      <c r="AT29" s="1"/>
+      <c r="AU29" s="1"/>
+      <c r="AV29" s="1"/>
+      <c r="AW29" s="1"/>
+      <c r="AX29" s="1"/>
+      <c r="AY29" s="1"/>
+      <c r="AZ29" s="1"/>
+      <c r="BA29" s="1"/>
+      <c r="BB29" s="1"/>
+      <c r="BC29" s="1"/>
+      <c r="BD29" s="1"/>
+      <c r="BE29" s="1"/>
+      <c r="BF29" s="1"/>
+      <c r="BG29" s="1"/>
+      <c r="BH29" s="1"/>
+      <c r="BI29" s="1"/>
+      <c r="BJ29" s="1"/>
+      <c r="BK29" s="1"/>
+      <c r="BL29" s="1"/>
+      <c r="BM29" s="1"/>
+      <c r="BN29" s="1"/>
+      <c r="BO29" s="1"/>
+      <c r="BP29" s="1"/>
+      <c r="BQ29" s="1"/>
+      <c r="BR29" s="1"/>
+      <c r="BS29" s="1"/>
+      <c r="BT29" s="1"/>
+      <c r="BU29" s="1"/>
+      <c r="BV29" s="1"/>
+      <c r="BW29" s="1"/>
+      <c r="BX29" s="1"/>
+      <c r="BY29" s="1"/>
+      <c r="BZ29" s="1"/>
+      <c r="CA29" s="1"/>
+      <c r="CB29" s="1"/>
+      <c r="CC29" s="1"/>
+      <c r="CD29" s="1"/>
+      <c r="CE29" s="1"/>
+      <c r="CF29" s="1"/>
+      <c r="CG29" s="1"/>
+      <c r="CH29" s="1"/>
+      <c r="CI29" s="1"/>
+      <c r="CJ29" s="1"/>
+      <c r="CK29" s="1"/>
+      <c r="CL29" s="1"/>
+      <c r="CM29" s="1"/>
+      <c r="CN29" s="1"/>
+      <c r="CO29" s="1"/>
+      <c r="CP29" s="1"/>
+      <c r="CQ29" s="1"/>
+      <c r="CR29" s="1"/>
+      <c r="CS29" s="1"/>
+      <c r="CT29" s="1"/>
+      <c r="CU29" s="1"/>
+      <c r="CV29" s="1"/>
+      <c r="CW29" s="1"/>
+      <c r="CX29" s="1"/>
+      <c r="CY29" s="1"/>
+      <c r="CZ29" s="1"/>
+      <c r="DA29" s="1"/>
+      <c r="DB29" s="1"/>
+      <c r="DC29" s="1"/>
+      <c r="DD29" s="1"/>
+      <c r="DE29" s="1"/>
+      <c r="DF29" s="1"/>
+      <c r="DG29" s="1"/>
+      <c r="DH29" s="1"/>
+      <c r="DI29" s="1"/>
+      <c r="DJ29" s="1"/>
+      <c r="DK29" s="1"/>
+      <c r="DL29" s="1"/>
+      <c r="DM29" s="1"/>
+      <c r="DN29" s="1"/>
+      <c r="DO29" s="1"/>
     </row>
     <row r="30" spans="1:119" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="1"/>
-      <c r="B30" s="1"/>
-      <c r="C30" s="1"/>
-      <c r="D30" s="1"/>
-      <c r="E30" s="1"/>
-      <c r="F30" s="1"/>
-      <c r="G30" s="1"/>
-      <c r="H30" s="1"/>
-      <c r="I30" s="1"/>
+      <c r="A30" s="64"/>
+      <c r="B30" s="64" t="s">
+        <v>306</v>
+      </c>
+      <c r="C30" s="64" t="s">
+        <v>260</v>
+      </c>
+      <c r="D30" s="64" t="s">
+        <v>8</v>
+      </c>
+      <c r="E30" s="67" t="s">
+        <v>12</v>
+      </c>
+      <c r="F30" s="70"/>
+      <c r="G30" s="68"/>
+      <c r="H30" s="64">
+        <v>401</v>
+      </c>
+      <c r="I30" s="64"/>
       <c r="J30" s="1"/>
       <c r="K30" s="1"/>
       <c r="L30" s="1"/>
@@ -3370,6 +3500,100 @@
       <c r="W30" s="1"/>
       <c r="X30" s="1"/>
       <c r="Y30" s="1"/>
+      <c r="Z30" s="1"/>
+      <c r="AA30" s="1"/>
+      <c r="AB30" s="1"/>
+      <c r="AC30" s="1"/>
+      <c r="AD30" s="1"/>
+      <c r="AE30" s="1"/>
+      <c r="AF30" s="1"/>
+      <c r="AG30" s="1"/>
+      <c r="AH30" s="1"/>
+      <c r="AI30" s="1"/>
+      <c r="AJ30" s="1"/>
+      <c r="AK30" s="1"/>
+      <c r="AL30" s="1"/>
+      <c r="AM30" s="1"/>
+      <c r="AN30" s="1"/>
+      <c r="AO30" s="1"/>
+      <c r="AP30" s="1"/>
+      <c r="AQ30" s="1"/>
+      <c r="AR30" s="1"/>
+      <c r="AS30" s="1"/>
+      <c r="AT30" s="1"/>
+      <c r="AU30" s="1"/>
+      <c r="AV30" s="1"/>
+      <c r="AW30" s="1"/>
+      <c r="AX30" s="1"/>
+      <c r="AY30" s="1"/>
+      <c r="AZ30" s="1"/>
+      <c r="BA30" s="1"/>
+      <c r="BB30" s="1"/>
+      <c r="BC30" s="1"/>
+      <c r="BD30" s="1"/>
+      <c r="BE30" s="1"/>
+      <c r="BF30" s="1"/>
+      <c r="BG30" s="1"/>
+      <c r="BH30" s="1"/>
+      <c r="BI30" s="1"/>
+      <c r="BJ30" s="1"/>
+      <c r="BK30" s="1"/>
+      <c r="BL30" s="1"/>
+      <c r="BM30" s="1"/>
+      <c r="BN30" s="1"/>
+      <c r="BO30" s="1"/>
+      <c r="BP30" s="1"/>
+      <c r="BQ30" s="1"/>
+      <c r="BR30" s="1"/>
+      <c r="BS30" s="1"/>
+      <c r="BT30" s="1"/>
+      <c r="BU30" s="1"/>
+      <c r="BV30" s="1"/>
+      <c r="BW30" s="1"/>
+      <c r="BX30" s="1"/>
+      <c r="BY30" s="1"/>
+      <c r="BZ30" s="1"/>
+      <c r="CA30" s="1"/>
+      <c r="CB30" s="1"/>
+      <c r="CC30" s="1"/>
+      <c r="CD30" s="1"/>
+      <c r="CE30" s="1"/>
+      <c r="CF30" s="1"/>
+      <c r="CG30" s="1"/>
+      <c r="CH30" s="1"/>
+      <c r="CI30" s="1"/>
+      <c r="CJ30" s="1"/>
+      <c r="CK30" s="1"/>
+      <c r="CL30" s="1"/>
+      <c r="CM30" s="1"/>
+      <c r="CN30" s="1"/>
+      <c r="CO30" s="1"/>
+      <c r="CP30" s="1"/>
+      <c r="CQ30" s="1"/>
+      <c r="CR30" s="1"/>
+      <c r="CS30" s="1"/>
+      <c r="CT30" s="1"/>
+      <c r="CU30" s="1"/>
+      <c r="CV30" s="1"/>
+      <c r="CW30" s="1"/>
+      <c r="CX30" s="1"/>
+      <c r="CY30" s="1"/>
+      <c r="CZ30" s="1"/>
+      <c r="DA30" s="1"/>
+      <c r="DB30" s="1"/>
+      <c r="DC30" s="1"/>
+      <c r="DD30" s="1"/>
+      <c r="DE30" s="1"/>
+      <c r="DF30" s="1"/>
+      <c r="DG30" s="1"/>
+      <c r="DH30" s="1"/>
+      <c r="DI30" s="1"/>
+      <c r="DJ30" s="1"/>
+      <c r="DK30" s="1"/>
+      <c r="DL30" s="1"/>
+      <c r="DM30" s="1"/>
+      <c r="DN30" s="1"/>
+      <c r="DO30" s="1"/>
     </row>
     <row r="31" spans="1:119" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="1"/>
@@ -28616,9 +28840,87 @@
       <c r="X965" s="1"/>
       <c r="Y965" s="1"/>
     </row>
-    <row r="966" spans="1:25" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="967" spans="1:25" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="968" spans="1:25" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="966" spans="1:25" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A966" s="1"/>
+      <c r="B966" s="1"/>
+      <c r="C966" s="1"/>
+      <c r="D966" s="1"/>
+      <c r="E966" s="1"/>
+      <c r="F966" s="1"/>
+      <c r="G966" s="1"/>
+      <c r="H966" s="1"/>
+      <c r="I966" s="1"/>
+      <c r="J966" s="1"/>
+      <c r="K966" s="1"/>
+      <c r="L966" s="1"/>
+      <c r="M966" s="1"/>
+      <c r="N966" s="1"/>
+      <c r="O966" s="1"/>
+      <c r="P966" s="1"/>
+      <c r="Q966" s="1"/>
+      <c r="R966" s="1"/>
+      <c r="S966" s="1"/>
+      <c r="T966" s="1"/>
+      <c r="U966" s="1"/>
+      <c r="V966" s="1"/>
+      <c r="W966" s="1"/>
+      <c r="X966" s="1"/>
+      <c r="Y966" s="1"/>
+    </row>
+    <row r="967" spans="1:25" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A967" s="1"/>
+      <c r="B967" s="1"/>
+      <c r="C967" s="1"/>
+      <c r="D967" s="1"/>
+      <c r="E967" s="1"/>
+      <c r="F967" s="1"/>
+      <c r="G967" s="1"/>
+      <c r="H967" s="1"/>
+      <c r="I967" s="1"/>
+      <c r="J967" s="1"/>
+      <c r="K967" s="1"/>
+      <c r="L967" s="1"/>
+      <c r="M967" s="1"/>
+      <c r="N967" s="1"/>
+      <c r="O967" s="1"/>
+      <c r="P967" s="1"/>
+      <c r="Q967" s="1"/>
+      <c r="R967" s="1"/>
+      <c r="S967" s="1"/>
+      <c r="T967" s="1"/>
+      <c r="U967" s="1"/>
+      <c r="V967" s="1"/>
+      <c r="W967" s="1"/>
+      <c r="X967" s="1"/>
+      <c r="Y967" s="1"/>
+    </row>
+    <row r="968" spans="1:25" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A968" s="1"/>
+      <c r="B968" s="1"/>
+      <c r="C968" s="1"/>
+      <c r="D968" s="1"/>
+      <c r="E968" s="1"/>
+      <c r="F968" s="1"/>
+      <c r="G968" s="1"/>
+      <c r="H968" s="1"/>
+      <c r="I968" s="1"/>
+      <c r="J968" s="1"/>
+      <c r="K968" s="1"/>
+      <c r="L968" s="1"/>
+      <c r="M968" s="1"/>
+      <c r="N968" s="1"/>
+      <c r="O968" s="1"/>
+      <c r="P968" s="1"/>
+      <c r="Q968" s="1"/>
+      <c r="R968" s="1"/>
+      <c r="S968" s="1"/>
+      <c r="T968" s="1"/>
+      <c r="U968" s="1"/>
+      <c r="V968" s="1"/>
+      <c r="W968" s="1"/>
+      <c r="X968" s="1"/>
+      <c r="Y968" s="1"/>
+    </row>
     <row r="969" spans="1:25" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="970" spans="1:25" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="971" spans="1:25" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -28646,13 +28948,12 @@
     <row r="993" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="994" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="995" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="996" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="997" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="998" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="F2" r:id="rId1" xr:uid="{3F9AAE22-B143-3242-A58F-C55E2A24C1B1}"/>
-    <hyperlink ref="F14" r:id="rId2" xr:uid="{DACCDA94-F617-FA49-B7CF-8C8EBFE78BB0}"/>
-    <hyperlink ref="F10" r:id="rId3" xr:uid="{F86BFBDD-9EBF-F048-87E2-22C083FE86D0}"/>
-    <hyperlink ref="F11:F13" r:id="rId4" display="dhuruvalak01@gmail.com" xr:uid="{6D346379-42AB-F741-90BB-79F8AE3F8D98}"/>
-    <hyperlink ref="F18" r:id="rId5" xr:uid="{A36D8596-FA7D-7540-84D3-6D80C05776CD}"/>
+    <hyperlink ref="G21" r:id="rId1" xr:uid="{6C5DA17E-080D-3F48-A6CE-8BA90C254F2C}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>
@@ -28732,7 +29033,7 @@
     </row>
     <row r="2" spans="1:28" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="48" t="s">
-        <v>286</v>
+        <v>282</v>
       </c>
       <c r="B2" s="49"/>
       <c r="C2" s="49"/>
@@ -28759,7 +29060,7 @@
       </c>
       <c r="E3" s="51"/>
       <c r="F3" s="51" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
       <c r="G3" s="51" t="s">
         <v>20</v>
@@ -28801,7 +29102,7 @@
         <v>400</v>
       </c>
       <c r="J4" s="51" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
     </row>
     <row r="5" spans="1:28" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -28819,7 +29120,7 @@
       </c>
       <c r="E5" s="51"/>
       <c r="F5" s="51" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
       <c r="G5" s="51" t="s">
         <v>20</v>
@@ -28849,7 +29150,7 @@
       </c>
       <c r="E6" s="51"/>
       <c r="F6" s="51" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
       <c r="G6" s="51"/>
       <c r="H6" s="51" t="s">
@@ -28883,12 +29184,12 @@
         <v>400</v>
       </c>
       <c r="J7" s="51" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
     </row>
     <row r="8" spans="1:28" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A8" s="50" t="s">
-        <v>292</v>
+        <v>288</v>
       </c>
       <c r="B8" s="51" t="s">
         <v>23</v>
@@ -28901,10 +29202,10 @@
       </c>
       <c r="E8" s="51"/>
       <c r="F8" s="51" t="s">
-        <v>293</v>
+        <v>289</v>
       </c>
       <c r="G8" s="51" t="s">
-        <v>294</v>
+        <v>290</v>
       </c>
       <c r="H8" s="51" t="s">
         <v>172</v>
@@ -28913,12 +29214,12 @@
         <v>400</v>
       </c>
       <c r="J8" s="51" t="s">
-        <v>295</v>
+        <v>291</v>
       </c>
     </row>
     <row r="9" spans="1:28" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A9" s="50" t="s">
-        <v>296</v>
+        <v>292</v>
       </c>
       <c r="B9" s="51" t="s">
         <v>23</v>
@@ -28941,7 +29242,7 @@
         <v>400</v>
       </c>
       <c r="J9" s="51" t="s">
-        <v>297</v>
+        <v>293</v>
       </c>
       <c r="K9" s="2"/>
       <c r="L9" s="2"/>
@@ -28977,7 +29278,7 @@
       </c>
       <c r="E10" s="51"/>
       <c r="F10" s="51" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
       <c r="G10" s="51">
         <v>123445</v>
@@ -28989,7 +29290,7 @@
         <v>400</v>
       </c>
       <c r="J10" s="51" t="s">
-        <v>297</v>
+        <v>293</v>
       </c>
       <c r="K10" s="2"/>
       <c r="L10" s="2"/>
@@ -29012,7 +29313,7 @@
     </row>
     <row r="11" spans="1:28" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A11" s="53" t="s">
-        <v>299</v>
+        <v>295</v>
       </c>
       <c r="B11" s="54" t="s">
         <v>23</v>
@@ -29025,10 +29326,10 @@
       </c>
       <c r="E11" s="54"/>
       <c r="F11" s="54" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
       <c r="G11" s="54" t="s">
-        <v>301</v>
+        <v>297</v>
       </c>
       <c r="H11" s="54" t="s">
         <v>21</v>
@@ -29129,7 +29430,7 @@
         <v>400</v>
       </c>
       <c r="J14" s="51" t="s">
-        <v>295</v>
+        <v>291</v>
       </c>
     </row>
     <row r="15" spans="1:28" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -29279,10 +29580,10 @@
       </c>
       <c r="E19" s="54"/>
       <c r="F19" s="54" t="s">
-        <v>302</v>
+        <v>298</v>
       </c>
       <c r="G19" s="54" t="s">
-        <v>303</v>
+        <v>299</v>
       </c>
       <c r="H19" s="54" t="s">
         <v>21</v>
@@ -29353,7 +29654,7 @@
         <v>404</v>
       </c>
       <c r="J21" s="51" t="s">
-        <v>304</v>
+        <v>300</v>
       </c>
     </row>
     <row r="22" spans="1:28" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -29381,7 +29682,7 @@
         <v>400</v>
       </c>
       <c r="J22" s="51" t="s">
-        <v>297</v>
+        <v>293</v>
       </c>
     </row>
     <row r="23" spans="1:28" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -29559,10 +29860,10 @@
       </c>
       <c r="E28" s="54"/>
       <c r="F28" s="54" t="s">
-        <v>302</v>
+        <v>298</v>
       </c>
       <c r="G28" s="54" t="s">
-        <v>305</v>
+        <v>301</v>
       </c>
       <c r="H28" s="54" t="s">
         <v>21</v>
@@ -29607,10 +29908,10 @@
       </c>
       <c r="E29" s="54"/>
       <c r="F29" s="54" t="s">
+        <v>298</v>
+      </c>
+      <c r="G29" s="54" t="s">
         <v>302</v>
-      </c>
-      <c r="G29" s="54" t="s">
-        <v>306</v>
       </c>
       <c r="H29" s="54" t="s">
         <v>56</v>
@@ -34467,10 +34768,10 @@
         <v>162</v>
       </c>
       <c r="O2" s="39" t="s">
-        <v>270</v>
+        <v>266</v>
       </c>
       <c r="P2" s="39" t="s">
-        <v>271</v>
+        <v>267</v>
       </c>
       <c r="Q2" s="40" t="s">
         <v>167</v>
@@ -34482,10 +34783,10 @@
         <v>164</v>
       </c>
       <c r="T2" s="41" t="s">
-        <v>272</v>
+        <v>268</v>
       </c>
       <c r="U2" s="39" t="s">
-        <v>273</v>
+        <v>269</v>
       </c>
       <c r="V2" s="39" t="s">
         <v>165</v>
@@ -34494,7 +34795,7 @@
         <v>166</v>
       </c>
       <c r="X2" s="41" t="s">
-        <v>274</v>
+        <v>270</v>
       </c>
       <c r="Y2" s="42"/>
       <c r="Z2" s="42"/>
@@ -34507,10 +34808,10 @@
     </row>
     <row r="3" spans="1:32" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="36" t="s">
-        <v>275</v>
+        <v>271</v>
       </c>
       <c r="B3" s="37" t="s">
-        <v>276</v>
+        <v>272</v>
       </c>
       <c r="C3" s="37" t="s">
         <v>8</v>
@@ -34549,10 +34850,10 @@
     </row>
     <row r="4" spans="1:32" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="36" t="s">
-        <v>277</v>
+        <v>273</v>
       </c>
       <c r="B4" s="37" t="s">
-        <v>278</v>
+        <v>274</v>
       </c>
       <c r="C4" s="37" t="s">
         <v>8</v>
@@ -34582,7 +34883,7 @@
       <c r="X4" s="37"/>
       <c r="Y4" s="37"/>
       <c r="Z4" s="37" t="s">
-        <v>279</v>
+        <v>275</v>
       </c>
       <c r="AA4" s="37"/>
       <c r="AB4" s="37"/>
@@ -34593,10 +34894,10 @@
     </row>
     <row r="5" spans="1:32" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A5" s="43" t="s">
-        <v>280</v>
+        <v>276</v>
       </c>
       <c r="B5" s="37" t="s">
-        <v>278</v>
+        <v>274</v>
       </c>
       <c r="C5" s="37" t="s">
         <v>8</v>
@@ -34626,7 +34927,7 @@
       <c r="X5" s="37"/>
       <c r="Y5" s="37"/>
       <c r="Z5" s="37" t="s">
-        <v>281</v>
+        <v>277</v>
       </c>
       <c r="AA5" s="37"/>
       <c r="AB5" s="37"/>
@@ -34637,10 +34938,10 @@
     </row>
     <row r="6" spans="1:32" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6" s="44" t="s">
-        <v>282</v>
+        <v>278</v>
       </c>
       <c r="B6" s="37" t="s">
-        <v>283</v>
+        <v>279</v>
       </c>
       <c r="C6" s="37" t="s">
         <v>8</v>
@@ -34669,7 +34970,7 @@
       <c r="W6" s="37"/>
       <c r="X6" s="37"/>
       <c r="Y6" s="37" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
       <c r="Z6" s="37"/>
       <c r="AA6" s="37"/>
@@ -34681,10 +34982,10 @@
     </row>
     <row r="7" spans="1:32" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="44" t="s">
-        <v>285</v>
+        <v>281</v>
       </c>
       <c r="B7" s="37" t="s">
-        <v>283</v>
+        <v>279</v>
       </c>
       <c r="C7" s="37" t="s">
         <v>8</v>

</xml_diff>